<commit_message>
v1.0.3: Settings page, BasePage refactor, configurable isotopic constants
- Add persistent Settings page (98_Settings.py) backed by user_settings.json
- Introduce BasePage class for consistent page setup (auth, config, sidebar)
- New modules: constants.py, config.py, filters.py, base_page.py
- Configurable isotopic constants and working-gas ratios via Settings
- Sanitize Session column in addition to Sample; block commas and semicolons
- Add 50°C equilibrated-gas target values for D47, D48, D49
- Remove deprecated calibration sets from init_params
- Remove 08_D47crunch_plots.py (merged elsewhere)
- Update SampleDatabase.xlsx with anonymized example data
- Refactor SessionStateManager to use shared db_connection
- Add render_plotly_chart helper in commons
</commit_message>
<xml_diff>
--- a/D4Xgui/static/SampleDatabase.xlsx
+++ b/D4Xgui/static/SampleDatabase.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10720"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mb_work/Desktop/software/PyCharm_1/D47crunch_GUI/static/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mb_work/PycharmProjects/D4Xgui_rev_SoftX/D4Xgui/static/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{189F2CDB-3C94-C845-95D9-A99E4CF41D46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{697B5767-B857-DC42-8164-51BCCB6FCBB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -199,38 +199,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -539,8 +517,8 @@
     <col min="1" max="1" width="22.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="41.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="40.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="46.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="40.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="46.1640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="24.83203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="37.1640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.6640625" bestFit="1" customWidth="1"/>

</xml_diff>